<commit_message>
Update dockerfiles and add publish script
Upstream tensorflow updated their dockerfiles/method of generating them.
This patchset used the new method to generate the dockerfiles, then
made minor changes. All the docker files had at least 1 `ARG` before
the `FROM` in order to select things like ubuntu or cuda versions. This
feature isn't supported until docker version >= 17.05.0, and rhel currently
has docker version 1.13.
</commit_message>
<xml_diff>
--- a/tensorflow/Dockerfiles/Final_license_list.xlsx
+++ b/tensorflow/Dockerfiles/Final_license_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\license_info\final_output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TaylorJakobson\Desktop\dev\build-scripts\tensorflow\Dockerfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4B943BCB-D806-46FE-96E7-20F89411D1C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9C7510B6-12CE-4950-A538-268911B12AE9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="625">
   <si>
     <t xml:space="preserve"> however there are some exceptions Example    Files: scripts/Dpkg/Gettext.pm is avialable under BSD-2-clause</t>
   </si>
@@ -1874,6 +1874,27 @@
   </si>
   <si>
     <t>libcudnn7-dev</t>
+  </si>
+  <si>
+    <t>pillow</t>
+  </si>
+  <si>
+    <t>matplotlib</t>
+  </si>
+  <si>
+    <t>scipy</t>
+  </si>
+  <si>
+    <t>sklearn</t>
+  </si>
+  <si>
+    <t>pandas</t>
+  </si>
+  <si>
+    <t>enum34</t>
+  </si>
+  <si>
+    <t>python-dev</t>
   </si>
 </sst>
 </file>
@@ -2714,10 +2735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP330"/>
+  <dimension ref="A1:BP337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="A276" sqref="A276"/>
+    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="A312" sqref="A312:XFD312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7814,86 +7835,107 @@
         <v>588</v>
       </c>
     </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>618</v>
+      </c>
+      <c r="B305" t="s">
+        <v>547</v>
+      </c>
+      <c r="C305" t="s">
+        <v>94</v>
+      </c>
+      <c r="D305" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>589</v>
+        <v>619</v>
+      </c>
+      <c r="B306" t="s">
+        <v>547</v>
+      </c>
+      <c r="C306" t="s">
+        <v>94</v>
       </c>
       <c r="D306" t="s">
-        <v>590</v>
-      </c>
-      <c r="E306" t="s">
-        <v>591</v>
+        <v>96</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>592</v>
+        <v>620</v>
+      </c>
+      <c r="B307" t="s">
+        <v>549</v>
+      </c>
+      <c r="C307" t="s">
+        <v>94</v>
       </c>
       <c r="D307" t="s">
-        <v>590</v>
-      </c>
-      <c r="E307" t="s">
-        <v>591</v>
+        <v>96</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>593</v>
+        <v>621</v>
+      </c>
+      <c r="B308" t="s">
+        <v>549</v>
+      </c>
+      <c r="C308" t="s">
+        <v>94</v>
       </c>
       <c r="D308" t="s">
-        <v>590</v>
-      </c>
-      <c r="E308" t="s">
-        <v>591</v>
+        <v>96</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>594</v>
+        <v>622</v>
+      </c>
+      <c r="B309" t="s">
+        <v>549</v>
+      </c>
+      <c r="C309" t="s">
+        <v>94</v>
       </c>
       <c r="D309" t="s">
-        <v>590</v>
-      </c>
-      <c r="E309" t="s">
-        <v>591</v>
+        <v>96</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>595</v>
+        <v>623</v>
+      </c>
+      <c r="B310" t="s">
+        <v>549</v>
+      </c>
+      <c r="C310" t="s">
+        <v>94</v>
       </c>
       <c r="D310" t="s">
-        <v>590</v>
-      </c>
-      <c r="E310" t="s">
-        <v>591</v>
+        <v>96</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>596</v>
+        <v>624</v>
+      </c>
+      <c r="B311" t="s">
+        <v>547</v>
+      </c>
+      <c r="C311" t="s">
+        <v>94</v>
       </c>
       <c r="D311" t="s">
-        <v>590</v>
-      </c>
-      <c r="E311" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
-        <v>597</v>
-      </c>
-      <c r="D312" t="s">
-        <v>590</v>
-      </c>
-      <c r="E312" t="s">
-        <v>591</v>
+        <v>96</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="D313" t="s">
         <v>590</v>
@@ -7904,7 +7946,7 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="D314" t="s">
         <v>590</v>
@@ -7915,7 +7957,7 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="D315" t="s">
         <v>590</v>
@@ -7926,7 +7968,7 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="D316" t="s">
         <v>590</v>
@@ -7937,7 +7979,7 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="D317" t="s">
         <v>590</v>
@@ -7948,7 +7990,7 @@
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="D318" t="s">
         <v>590</v>
@@ -7959,7 +8001,7 @@
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="D319" t="s">
         <v>590</v>
@@ -7970,7 +8012,7 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="D320" t="s">
         <v>590</v>
@@ -7981,7 +8023,7 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="D321" t="s">
         <v>590</v>
@@ -7992,7 +8034,7 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="D322" t="s">
         <v>590</v>
@@ -8003,7 +8045,7 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="D323" t="s">
         <v>590</v>
@@ -8014,7 +8056,7 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="D324" t="s">
         <v>590</v>
@@ -8025,7 +8067,7 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="D325" t="s">
         <v>590</v>
@@ -8036,7 +8078,7 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="D326" t="s">
         <v>590</v>
@@ -8047,7 +8089,7 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="D327" t="s">
         <v>590</v>
@@ -8058,7 +8100,7 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="D328" t="s">
         <v>590</v>
@@ -8069,23 +8111,100 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="D329" t="s">
-        <v>615</v>
+        <v>590</v>
       </c>
       <c r="E329" t="s">
-        <v>616</v>
+        <v>591</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
+        <v>608</v>
+      </c>
+      <c r="D330" t="s">
+        <v>590</v>
+      </c>
+      <c r="E330" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>609</v>
+      </c>
+      <c r="D331" t="s">
+        <v>590</v>
+      </c>
+      <c r="E331" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>610</v>
+      </c>
+      <c r="D332" t="s">
+        <v>590</v>
+      </c>
+      <c r="E332" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>611</v>
+      </c>
+      <c r="D333" t="s">
+        <v>590</v>
+      </c>
+      <c r="E333" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>612</v>
+      </c>
+      <c r="D334" t="s">
+        <v>590</v>
+      </c>
+      <c r="E334" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>613</v>
+      </c>
+      <c r="D335" t="s">
+        <v>590</v>
+      </c>
+      <c r="E335" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>614</v>
+      </c>
+      <c r="D336" t="s">
+        <v>615</v>
+      </c>
+      <c r="E336" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
         <v>617</v>
       </c>
-      <c r="D330" t="s">
+      <c r="D337" t="s">
         <v>615</v>
       </c>
-      <c r="E330" t="s">
+      <c r="E337" t="s">
         <v>616</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add headers to Final_license_list spreadshet
</commit_message>
<xml_diff>
--- a/tensorflow/Dockerfiles/Final_license_list.xlsx
+++ b/tensorflow/Dockerfiles/Final_license_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TaylorJakobson\Desktop\dev\build-scripts\tensorflow\Dockerfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{11DB8979-4C74-435E-A30D-4402F972AD99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DE3B1C-7255-44EA-B6EE-CA8F96745762}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3337" uniqueCount="525">
   <si>
     <t xml:space="preserve"> however there are some exceptions Example    Files: scripts/Dpkg/Gettext.pm is avialable under BSD-2-clause</t>
   </si>
@@ -1586,13 +1586,22 @@
   </si>
   <si>
     <t>python-dev</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>License/Copyright Links/References</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1734,6 +1743,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2078,9 +2094,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2437,10 +2455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN335"/>
+  <dimension ref="A1:BN336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,22 +2469,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" t="s">
-        <v>94</v>
+      <c r="A1" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
@@ -2474,10 +2492,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
@@ -2485,7 +2503,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>98</v>
@@ -2496,7 +2514,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
         <v>98</v>
@@ -2507,10 +2525,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
         <v>94</v>
@@ -2518,10 +2536,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>94</v>
@@ -2529,10 +2547,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
         <v>94</v>
@@ -2540,10 +2558,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>94</v>
@@ -2551,10 +2569,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
         <v>94</v>
@@ -2562,10 +2580,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>94</v>
@@ -2573,10 +2591,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
         <v>94</v>
@@ -2584,7 +2602,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
         <v>110</v>
@@ -2595,10 +2613,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
         <v>94</v>
@@ -2606,7 +2624,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -2617,10 +2635,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
         <v>94</v>
@@ -2628,10 +2646,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
         <v>94</v>
@@ -2639,10 +2657,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
         <v>94</v>
@@ -2650,10 +2668,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
         <v>94</v>
@@ -2661,10 +2679,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
         <v>94</v>
@@ -2672,10 +2690,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
         <v>94</v>
@@ -2683,7 +2701,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
         <v>93</v>
@@ -2694,10 +2712,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
         <v>94</v>
@@ -2705,10 +2723,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
         <v>94</v>
@@ -2716,10 +2734,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
         <v>94</v>
@@ -2727,10 +2745,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="C26" t="s">
         <v>94</v>
@@ -2738,10 +2756,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C27" t="s">
         <v>94</v>
@@ -2749,10 +2767,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C28" t="s">
         <v>94</v>
@@ -2760,10 +2778,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
         <v>94</v>
@@ -2771,10 +2789,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
         <v>94</v>
@@ -2782,10 +2800,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>134</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
         <v>94</v>
@@ -2793,10 +2811,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>134</v>
       </c>
       <c r="C32" t="s">
         <v>94</v>
@@ -2804,10 +2822,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
         <v>94</v>
@@ -2815,10 +2833,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
         <v>94</v>
@@ -2826,10 +2844,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
         <v>94</v>
@@ -2837,10 +2855,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
         <v>94</v>
@@ -2848,10 +2866,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
         <v>94</v>
@@ -2859,10 +2877,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="C38" t="s">
         <v>94</v>
@@ -2870,10 +2888,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="C39" t="s">
         <v>94</v>
@@ -2881,10 +2899,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
         <v>94</v>
@@ -2892,10 +2910,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
         <v>94</v>
@@ -2903,7 +2921,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
         <v>96</v>
@@ -2914,7 +2932,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B43" t="s">
         <v>96</v>
@@ -2925,7 +2943,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B44" t="s">
         <v>96</v>
@@ -2936,10 +2954,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C45" t="s">
         <v>94</v>
@@ -2947,10 +2965,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C46" t="s">
         <v>94</v>
@@ -2958,10 +2976,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
         <v>94</v>
@@ -2969,10 +2987,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C48" t="s">
         <v>94</v>
@@ -2980,7 +2998,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" t="s">
         <v>96</v>
@@ -2991,7 +3009,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B50" t="s">
         <v>96</v>
@@ -3002,7 +3020,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
         <v>96</v>
@@ -3013,7 +3031,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
         <v>96</v>
@@ -3024,7 +3042,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
         <v>96</v>
@@ -3035,7 +3053,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B54" t="s">
         <v>96</v>
@@ -3046,7 +3064,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B55" t="s">
         <v>96</v>
@@ -3057,10 +3075,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
         <v>94</v>
@@ -3068,10 +3086,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="C57" t="s">
         <v>94</v>
@@ -3079,10 +3097,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C58" t="s">
         <v>94</v>
@@ -3090,10 +3108,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
         <v>94</v>
@@ -3101,10 +3119,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B60" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
         <v>94</v>
@@ -3112,10 +3130,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B61" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
         <v>94</v>
@@ -3123,10 +3141,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>167</v>
       </c>
       <c r="C62" t="s">
         <v>94</v>
@@ -3134,10 +3152,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B63" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C63" t="s">
         <v>94</v>
@@ -3145,7 +3163,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B64" t="s">
         <v>98</v>
@@ -3156,10 +3174,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B65" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C65" t="s">
         <v>94</v>
@@ -3167,10 +3185,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B66" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C66" t="s">
         <v>94</v>
@@ -3178,10 +3196,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>110</v>
       </c>
       <c r="C67" t="s">
         <v>94</v>
@@ -3189,10 +3207,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="C68" t="s">
         <v>94</v>
@@ -3200,10 +3218,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B69" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="C69" t="s">
         <v>94</v>
@@ -3211,10 +3229,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>176</v>
       </c>
       <c r="C70" t="s">
         <v>94</v>
@@ -3222,7 +3240,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B71" t="s">
         <v>96</v>
@@ -3233,10 +3251,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B72" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="C72" t="s">
         <v>94</v>
@@ -3244,10 +3262,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="C73" t="s">
         <v>94</v>
@@ -3255,10 +3273,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B74" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C74" t="s">
         <v>94</v>
@@ -3266,10 +3284,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B75" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C75" t="s">
         <v>94</v>
@@ -3277,10 +3295,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B76" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="C76" t="s">
         <v>94</v>
@@ -3288,10 +3306,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="C77" t="s">
         <v>94</v>
@@ -3299,10 +3317,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B78" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C78" t="s">
         <v>94</v>
@@ -3310,10 +3328,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B79" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C79" t="s">
         <v>94</v>
@@ -3321,10 +3339,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B80" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C80" t="s">
         <v>94</v>
@@ -3332,95 +3350,98 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>187</v>
+      </c>
+      <c r="B81" t="s">
+        <v>98</v>
+      </c>
+      <c r="C81" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>188</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>96</v>
       </c>
-      <c r="C81" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>189</v>
-      </c>
-      <c r="B83" t="s">
-        <v>190</v>
-      </c>
-      <c r="C83" t="s">
-        <v>192</v>
+      <c r="C82" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B84" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C84" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B85" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C85" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B86" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C86" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B87" t="s">
-        <v>202</v>
-      </c>
-      <c r="D87" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87" t="s">
-        <v>1</v>
+        <v>199</v>
+      </c>
+      <c r="C87" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B88" t="s">
-        <v>204</v>
-      </c>
-      <c r="C88" t="s">
-        <v>205</v>
+        <v>202</v>
+      </c>
+      <c r="D88" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B89" t="s">
-        <v>207</v>
+        <v>204</v>
+      </c>
+      <c r="C89" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B90" t="s">
         <v>207</v>
@@ -3428,18 +3449,15 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B91" t="s">
-        <v>199</v>
-      </c>
-      <c r="C91" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B92" t="s">
         <v>199</v>
@@ -3450,97 +3468,97 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B93" t="s">
-        <v>212</v>
+        <v>199</v>
+      </c>
+      <c r="C93" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B94" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B95" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
-      </c>
-      <c r="C96" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B97" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C97" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B98" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="C98" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B99" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="C99" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B100" t="s">
         <v>223</v>
       </c>
       <c r="C100" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B101" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C101" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B102" t="s">
         <v>228</v>
@@ -3551,29 +3569,29 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B103" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="C103" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B104" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
       <c r="C104" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B105" t="s">
         <v>232</v>
@@ -3584,7 +3602,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B106" t="s">
         <v>232</v>
@@ -3595,32 +3613,32 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B107" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C107" t="s">
-        <v>237</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B108" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C108" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B109" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C109" t="s">
         <v>191</v>
@@ -3628,37 +3646,37 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B110" t="s">
-        <v>199</v>
+        <v>241</v>
       </c>
       <c r="C110" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B111" t="s">
-        <v>212</v>
+        <v>199</v>
+      </c>
+      <c r="C111" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B112" t="s">
-        <v>245</v>
-      </c>
-      <c r="C112" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B113" t="s">
         <v>245</v>
@@ -3669,56 +3687,56 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B114" t="s">
-        <v>248</v>
+        <v>245</v>
+      </c>
+      <c r="C114" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B115" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B116" t="s">
-        <v>252</v>
-      </c>
-      <c r="C116" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B117" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C117" t="s">
-        <v>255</v>
+        <v>191</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B118" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="C118" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B119" t="s">
         <v>245</v>
@@ -3729,7 +3747,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B120" t="s">
         <v>245</v>
@@ -3740,51 +3758,51 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B121" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="C121" t="s">
-        <v>191</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B122" t="s">
-        <v>263</v>
+        <v>261</v>
+      </c>
+      <c r="C122" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B123" t="s">
-        <v>265</v>
-      </c>
-      <c r="C123" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B124" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C124" t="s">
-        <v>191</v>
+        <v>266</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B125" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C125" t="s">
         <v>191</v>
@@ -3792,10 +3810,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B126" t="s">
-        <v>204</v>
+        <v>270</v>
       </c>
       <c r="C126" t="s">
         <v>191</v>
@@ -3803,59 +3821,59 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B127" t="s">
-        <v>273</v>
+        <v>204</v>
+      </c>
+      <c r="C127" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B128" t="s">
-        <v>275</v>
-      </c>
-      <c r="C128" t="s">
-        <v>191</v>
+        <v>273</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B129" t="s">
-        <v>199</v>
+        <v>275</v>
       </c>
       <c r="C129" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B130" t="s">
         <v>199</v>
       </c>
       <c r="C130" t="s">
-        <v>278</v>
+        <v>200</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B131" t="s">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="C131" t="s">
-        <v>191</v>
+        <v>278</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B132" t="s">
         <v>241</v>
@@ -3866,10 +3884,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B133" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C133" t="s">
         <v>191</v>
@@ -3877,37 +3895,37 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B134" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="C134" t="s">
-        <v>283</v>
+        <v>191</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B135" t="s">
-        <v>212</v>
+        <v>245</v>
+      </c>
+      <c r="C135" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B136" t="s">
-        <v>245</v>
-      </c>
-      <c r="C136" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B137" t="s">
         <v>245</v>
@@ -3918,7 +3936,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B138" t="s">
         <v>245</v>
@@ -3929,40 +3947,40 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B139" t="s">
-        <v>289</v>
+        <v>245</v>
+      </c>
+      <c r="C139" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B140" t="s">
-        <v>199</v>
-      </c>
-      <c r="C140" t="s">
-        <v>200</v>
+        <v>289</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B141" t="s">
-        <v>292</v>
+        <v>199</v>
       </c>
       <c r="C141" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B142" t="s">
-        <v>220</v>
+        <v>292</v>
       </c>
       <c r="C142" t="s">
         <v>191</v>
@@ -3970,32 +3988,32 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B143" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C143" t="s">
-        <v>295</v>
+        <v>191</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B144" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C144" t="s">
-        <v>191</v>
+        <v>295</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B145" t="s">
-        <v>268</v>
+        <v>220</v>
       </c>
       <c r="C145" t="s">
         <v>191</v>
@@ -4003,10 +4021,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B146" t="s">
-        <v>299</v>
+        <v>268</v>
       </c>
       <c r="C146" t="s">
         <v>191</v>
@@ -4014,10 +4032,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B147" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C147" t="s">
         <v>191</v>
@@ -4025,26 +4043,26 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B148" t="s">
-        <v>303</v>
+        <v>301</v>
+      </c>
+      <c r="C148" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B149" t="s">
-        <v>245</v>
-      </c>
-      <c r="C149" t="s">
-        <v>191</v>
+        <v>303</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B150" t="s">
         <v>245</v>
@@ -4055,10 +4073,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B151" t="s">
-        <v>307</v>
+        <v>245</v>
       </c>
       <c r="C151" t="s">
         <v>191</v>
@@ -4066,40 +4084,40 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B152" t="s">
-        <v>309</v>
+        <v>307</v>
+      </c>
+      <c r="C152" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B153" t="s">
-        <v>199</v>
-      </c>
-      <c r="C153" t="s">
-        <v>200</v>
+        <v>309</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B154" t="s">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="C154" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B155" t="s">
-        <v>313</v>
+        <v>241</v>
       </c>
       <c r="C155" t="s">
         <v>191</v>
@@ -4107,7 +4125,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B156" t="s">
         <v>313</v>
@@ -4118,7 +4136,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B157" t="s">
         <v>313</v>
@@ -4129,7 +4147,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B158" t="s">
         <v>313</v>
@@ -4140,7 +4158,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B159" t="s">
         <v>313</v>
@@ -4151,10 +4169,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B160" t="s">
-        <v>245</v>
+        <v>313</v>
       </c>
       <c r="C160" t="s">
         <v>191</v>
@@ -4162,67 +4180,67 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B161" t="s">
-        <v>309</v>
+        <v>245</v>
+      </c>
+      <c r="C161" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B162" t="s">
-        <v>321</v>
-      </c>
-      <c r="C162" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B163" t="s">
-        <v>324</v>
+        <v>321</v>
+      </c>
+      <c r="C163" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B164" t="s">
-        <v>326</v>
-      </c>
-      <c r="C164" t="s">
-        <v>191</v>
+        <v>324</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B165" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C165" t="s">
-        <v>329</v>
+        <v>191</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B166" t="s">
         <v>328</v>
       </c>
       <c r="C166" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B167" t="s">
         <v>328</v>
@@ -4233,21 +4251,21 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B168" t="s">
-        <v>232</v>
+        <v>328</v>
       </c>
       <c r="C168" t="s">
-        <v>191</v>
+        <v>331</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B169" t="s">
-        <v>335</v>
+        <v>232</v>
       </c>
       <c r="C169" t="s">
         <v>191</v>
@@ -4255,7 +4273,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B170" t="s">
         <v>335</v>
@@ -4266,7 +4284,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B171" t="s">
         <v>335</v>
@@ -4277,10 +4295,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B172" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C172" t="s">
         <v>191</v>
@@ -4288,10 +4306,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B173" t="s">
-        <v>245</v>
+        <v>339</v>
       </c>
       <c r="C173" t="s">
         <v>191</v>
@@ -4299,10 +4317,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B174" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="C174" t="s">
         <v>191</v>
@@ -4310,10 +4328,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B175" t="s">
-        <v>343</v>
+        <v>232</v>
       </c>
       <c r="C175" t="s">
         <v>191</v>
@@ -4321,10 +4339,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B176" t="s">
-        <v>245</v>
+        <v>343</v>
       </c>
       <c r="C176" t="s">
         <v>191</v>
@@ -4332,48 +4350,48 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B177" t="s">
         <v>245</v>
       </c>
       <c r="C177" t="s">
-        <v>346</v>
+        <v>191</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B178" t="s">
-        <v>348</v>
+        <v>245</v>
       </c>
       <c r="C178" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B179" t="s">
-        <v>351</v>
+        <v>348</v>
+      </c>
+      <c r="C179" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B180" t="s">
-        <v>292</v>
-      </c>
-      <c r="C180" t="s">
-        <v>191</v>
+        <v>351</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B181" t="s">
         <v>292</v>
@@ -4384,26 +4402,26 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B182" t="s">
-        <v>355</v>
+        <v>292</v>
+      </c>
+      <c r="C182" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B183" t="s">
-        <v>292</v>
-      </c>
-      <c r="C183" t="s">
-        <v>191</v>
+        <v>355</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B184" t="s">
         <v>292</v>
@@ -4414,29 +4432,29 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B185" t="s">
-        <v>359</v>
+        <v>292</v>
       </c>
       <c r="C185" t="s">
-        <v>360</v>
+        <v>191</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B186" t="s">
-        <v>245</v>
+        <v>359</v>
       </c>
       <c r="C186" t="s">
-        <v>191</v>
+        <v>360</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B187" t="s">
         <v>245</v>
@@ -4447,92 +4465,92 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B188" t="s">
-        <v>321</v>
+        <v>245</v>
       </c>
       <c r="C188" t="s">
-        <v>364</v>
+        <v>191</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B189" t="s">
-        <v>366</v>
+        <v>321</v>
       </c>
       <c r="C189" t="s">
-        <v>191</v>
+        <v>364</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B190" t="s">
-        <v>368</v>
+        <v>366</v>
+      </c>
+      <c r="C190" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B191" t="s">
-        <v>223</v>
-      </c>
-      <c r="C191" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B192" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
       <c r="C192" t="s">
-        <v>191</v>
+        <v>370</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B193" t="s">
-        <v>373</v>
+        <v>245</v>
       </c>
       <c r="C193" t="s">
-        <v>374</v>
+        <v>191</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B194" t="s">
-        <v>199</v>
+        <v>373</v>
       </c>
       <c r="C194" t="s">
-        <v>200</v>
+        <v>374</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B195" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
       <c r="C195" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B196" t="s">
         <v>232</v>
@@ -4543,29 +4561,29 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B197" t="s">
-        <v>379</v>
+        <v>232</v>
       </c>
       <c r="C197" t="s">
-        <v>380</v>
+        <v>191</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B198" t="s">
-        <v>245</v>
+        <v>379</v>
       </c>
       <c r="C198" t="s">
-        <v>191</v>
+        <v>380</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B199" t="s">
         <v>245</v>
@@ -4576,7 +4594,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B200" t="s">
         <v>245</v>
@@ -4587,7 +4605,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B201" t="s">
         <v>245</v>
@@ -4598,7 +4616,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B202" t="s">
         <v>245</v>
@@ -4609,7 +4627,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B203" t="s">
         <v>245</v>
@@ -4620,7 +4638,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B204" t="s">
         <v>245</v>
@@ -4631,7 +4649,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B205" t="s">
         <v>245</v>
@@ -4642,7 +4660,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B206" t="s">
         <v>245</v>
@@ -4653,7 +4671,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B207" t="s">
         <v>245</v>
@@ -4664,7 +4682,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B208" t="s">
         <v>245</v>
@@ -4675,7 +4693,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B209" t="s">
         <v>245</v>
@@ -4686,7 +4704,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B210" t="s">
         <v>245</v>
@@ -4697,7 +4715,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B211" t="s">
         <v>245</v>
@@ -4708,7 +4726,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B212" t="s">
         <v>245</v>
@@ -4719,7 +4737,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B213" t="s">
         <v>245</v>
@@ -4730,10 +4748,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B214" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="C214" t="s">
         <v>191</v>
@@ -4741,18 +4759,18 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B215" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="C215" t="s">
-        <v>399</v>
+        <v>191</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B216" t="s">
         <v>245</v>
@@ -4763,18 +4781,18 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B217" t="s">
         <v>245</v>
       </c>
       <c r="C217" t="s">
-        <v>191</v>
+        <v>399</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B218" t="s">
         <v>245</v>
@@ -4785,7 +4803,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B219" t="s">
         <v>245</v>
@@ -4796,10 +4814,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B220" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="C220" t="s">
         <v>191</v>
@@ -4807,7 +4825,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B221" t="s">
         <v>270</v>
@@ -4818,7 +4836,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B222" t="s">
         <v>270</v>
@@ -4829,10 +4847,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B223" t="s">
-        <v>408</v>
+        <v>270</v>
       </c>
       <c r="C223" t="s">
         <v>191</v>
@@ -4840,7 +4858,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B224" t="s">
         <v>408</v>
@@ -4851,32 +4869,32 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B225" t="s">
-        <v>245</v>
+        <v>408</v>
       </c>
       <c r="C225" t="s">
-        <v>399</v>
+        <v>191</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B226" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="C226" t="s">
-        <v>191</v>
+        <v>399</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B227" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="C227" t="s">
         <v>191</v>
@@ -4884,7 +4902,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B228" t="s">
         <v>245</v>
@@ -4895,32 +4913,32 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B229" t="s">
         <v>245</v>
       </c>
       <c r="C229" t="s">
-        <v>399</v>
+        <v>191</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B230" t="s">
-        <v>416</v>
+        <v>245</v>
       </c>
       <c r="C230" t="s">
-        <v>191</v>
+        <v>399</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B231" t="s">
-        <v>239</v>
+        <v>416</v>
       </c>
       <c r="C231" t="s">
         <v>191</v>
@@ -4928,10 +4946,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B232" t="s">
-        <v>299</v>
+        <v>239</v>
       </c>
       <c r="C232" t="s">
         <v>191</v>
@@ -4939,10 +4957,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B233" t="s">
-        <v>420</v>
+        <v>299</v>
       </c>
       <c r="C233" t="s">
         <v>191</v>
@@ -4950,10 +4968,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B234" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C234" t="s">
         <v>191</v>
@@ -4961,10 +4979,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B235" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C235" t="s">
         <v>191</v>
@@ -4972,10 +4990,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B236" t="s">
-        <v>241</v>
+        <v>424</v>
       </c>
       <c r="C236" t="s">
         <v>191</v>
@@ -4983,26 +5001,26 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B237" t="s">
-        <v>351</v>
+        <v>241</v>
+      </c>
+      <c r="C237" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B238" t="s">
-        <v>292</v>
-      </c>
-      <c r="C238" t="s">
-        <v>191</v>
+        <v>351</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B239" t="s">
         <v>292</v>
@@ -5013,7 +5031,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B240" t="s">
         <v>292</v>
@@ -5024,32 +5042,32 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B241" t="s">
-        <v>241</v>
+        <v>292</v>
       </c>
       <c r="C241" t="s">
-        <v>431</v>
+        <v>191</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B242" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C242" t="s">
-        <v>191</v>
+        <v>431</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B243" t="s">
-        <v>321</v>
+        <v>245</v>
       </c>
       <c r="C243" t="s">
         <v>191</v>
@@ -5057,10 +5075,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B244" t="s">
-        <v>292</v>
+        <v>321</v>
       </c>
       <c r="C244" t="s">
         <v>191</v>
@@ -5068,10 +5086,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B245" t="s">
-        <v>236</v>
+        <v>292</v>
       </c>
       <c r="C245" t="s">
         <v>191</v>
@@ -5079,10 +5097,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B246" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C246" t="s">
         <v>191</v>
@@ -5090,10 +5108,10 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B247" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C247" t="s">
         <v>191</v>
@@ -5101,10 +5119,10 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B248" t="s">
-        <v>292</v>
+        <v>241</v>
       </c>
       <c r="C248" t="s">
         <v>191</v>
@@ -5112,7 +5130,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B249" t="s">
         <v>292</v>
@@ -5123,62 +5141,62 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B250" t="s">
-        <v>241</v>
+        <v>292</v>
       </c>
       <c r="C250" t="s">
-        <v>441</v>
+        <v>191</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B251" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C251" t="s">
-        <v>191</v>
+        <v>441</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B252" t="s">
-        <v>379</v>
+        <v>245</v>
       </c>
       <c r="C252" t="s">
-        <v>380</v>
+        <v>191</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B253" t="s">
-        <v>245</v>
+        <v>379</v>
       </c>
       <c r="C253" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B254" t="s">
         <v>245</v>
       </c>
       <c r="C254" t="s">
-        <v>191</v>
+        <v>399</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B255" t="s">
         <v>245</v>
@@ -5189,7 +5207,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B256" t="s">
         <v>245</v>
@@ -5200,29 +5218,29 @@
     </row>
     <row r="257" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B257" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C257" t="s">
-        <v>449</v>
+        <v>191</v>
       </c>
     </row>
     <row r="258" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B258" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C258" t="s">
-        <v>191</v>
+        <v>449</v>
       </c>
     </row>
     <row r="259" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B259" t="s">
         <v>245</v>
@@ -5233,466 +5251,466 @@
     </row>
     <row r="260" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B260" t="s">
-        <v>289</v>
+        <v>245</v>
+      </c>
+      <c r="C260" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="261" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B261" t="s">
-        <v>454</v>
-      </c>
-      <c r="C261" t="s">
-        <v>191</v>
+        <v>289</v>
       </c>
     </row>
     <row r="262" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
+        <v>453</v>
+      </c>
+      <c r="B262" t="s">
+        <v>454</v>
+      </c>
+      <c r="C262" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="263" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
         <v>455</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B263" t="s">
         <v>408</v>
       </c>
-      <c r="C262" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="264" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>456</v>
-      </c>
-      <c r="B264" t="s">
-        <v>457</v>
+      <c r="C263" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="265" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B265" t="s">
-        <v>459</v>
-      </c>
-      <c r="D265" t="s">
-        <v>5</v>
-      </c>
-      <c r="E265" t="s">
-        <v>6</v>
-      </c>
-      <c r="F265" t="s">
-        <v>7</v>
-      </c>
-      <c r="G265" t="s">
-        <v>8</v>
-      </c>
-      <c r="H265" t="s">
-        <v>9</v>
-      </c>
-      <c r="I265" t="s">
-        <v>10</v>
-      </c>
-      <c r="J265" t="s">
-        <v>11</v>
-      </c>
-      <c r="K265" t="s">
-        <v>12</v>
-      </c>
-      <c r="L265" t="s">
-        <v>13</v>
-      </c>
-      <c r="M265" t="s">
-        <v>14</v>
-      </c>
-      <c r="N265" t="s">
-        <v>15</v>
-      </c>
-      <c r="O265" t="s">
-        <v>16</v>
-      </c>
-      <c r="P265" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q265" t="s">
-        <v>18</v>
-      </c>
-      <c r="R265" t="s">
-        <v>19</v>
-      </c>
-      <c r="S265" t="s">
-        <v>20</v>
-      </c>
-      <c r="T265" t="s">
-        <v>21</v>
-      </c>
-      <c r="U265" t="s">
-        <v>22</v>
-      </c>
-      <c r="V265" t="s">
-        <v>23</v>
-      </c>
-      <c r="W265" t="s">
-        <v>24</v>
-      </c>
-      <c r="X265" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y265" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z265" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA265" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB265" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC265" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD265" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE265" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF265" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG265" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH265" t="s">
-        <v>3</v>
+        <v>457</v>
       </c>
     </row>
     <row r="266" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B266" t="s">
-        <v>461</v>
+        <v>459</v>
+      </c>
+      <c r="D266" t="s">
+        <v>5</v>
+      </c>
+      <c r="E266" t="s">
+        <v>6</v>
+      </c>
+      <c r="F266" t="s">
+        <v>7</v>
+      </c>
+      <c r="G266" t="s">
+        <v>8</v>
+      </c>
+      <c r="H266" t="s">
+        <v>9</v>
+      </c>
+      <c r="I266" t="s">
+        <v>10</v>
+      </c>
+      <c r="J266" t="s">
+        <v>11</v>
+      </c>
+      <c r="K266" t="s">
+        <v>12</v>
+      </c>
+      <c r="L266" t="s">
+        <v>13</v>
+      </c>
+      <c r="M266" t="s">
+        <v>14</v>
+      </c>
+      <c r="N266" t="s">
+        <v>15</v>
+      </c>
+      <c r="O266" t="s">
+        <v>16</v>
+      </c>
+      <c r="P266" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q266" t="s">
+        <v>18</v>
+      </c>
+      <c r="R266" t="s">
+        <v>19</v>
+      </c>
+      <c r="S266" t="s">
+        <v>20</v>
+      </c>
+      <c r="T266" t="s">
+        <v>21</v>
+      </c>
+      <c r="U266" t="s">
+        <v>22</v>
+      </c>
+      <c r="V266" t="s">
+        <v>23</v>
+      </c>
+      <c r="W266" t="s">
+        <v>24</v>
+      </c>
+      <c r="X266" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y266" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z266" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA266" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB266" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC266" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD266" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE266" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF266" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG266" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH266" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="267" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B267" t="s">
-        <v>463</v>
-      </c>
-      <c r="D267" t="s">
-        <v>36</v>
-      </c>
-      <c r="E267" t="s">
-        <v>35</v>
-      </c>
-      <c r="F267" t="s">
-        <v>37</v>
-      </c>
-      <c r="G267" t="s">
-        <v>38</v>
-      </c>
-      <c r="H267" t="s">
-        <v>39</v>
-      </c>
-      <c r="I267" t="s">
-        <v>40</v>
-      </c>
-      <c r="J267" t="s">
-        <v>41</v>
-      </c>
-      <c r="K267" t="s">
-        <v>42</v>
-      </c>
-      <c r="L267" t="s">
-        <v>43</v>
-      </c>
-      <c r="M267" t="s">
-        <v>44</v>
-      </c>
-      <c r="N267" t="s">
-        <v>45</v>
-      </c>
-      <c r="O267" t="s">
-        <v>35</v>
-      </c>
-      <c r="P267" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q267" t="s">
-        <v>47</v>
-      </c>
-      <c r="R267" t="s">
-        <v>48</v>
-      </c>
-      <c r="S267" t="s">
-        <v>49</v>
-      </c>
-      <c r="T267" t="s">
-        <v>50</v>
-      </c>
-      <c r="U267" t="s">
-        <v>51</v>
-      </c>
-      <c r="V267" t="s">
-        <v>9</v>
-      </c>
-      <c r="W267" t="s">
-        <v>52</v>
-      </c>
-      <c r="X267" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y267" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z267" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA267" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB267" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC267" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD267" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE267" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF267" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG267" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH267" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI267" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ267" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK267" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL267" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM267" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN267" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO267" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP267" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ267" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR267" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS267" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT267" t="s">
-        <v>75</v>
-      </c>
-      <c r="AU267" t="s">
-        <v>76</v>
-      </c>
-      <c r="AV267" t="s">
-        <v>77</v>
-      </c>
-      <c r="AW267" t="s">
-        <v>78</v>
-      </c>
-      <c r="AX267" t="s">
-        <v>50</v>
-      </c>
-      <c r="AY267" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ267" t="s">
-        <v>80</v>
-      </c>
-      <c r="BA267" t="s">
-        <v>81</v>
-      </c>
-      <c r="BB267" t="s">
-        <v>82</v>
-      </c>
-      <c r="BC267" t="s">
-        <v>83</v>
-      </c>
-      <c r="BD267" t="s">
-        <v>84</v>
-      </c>
-      <c r="BE267" t="s">
-        <v>85</v>
-      </c>
-      <c r="BF267" t="s">
-        <v>86</v>
-      </c>
-      <c r="BG267" t="s">
-        <v>87</v>
-      </c>
-      <c r="BH267" t="s">
-        <v>88</v>
-      </c>
-      <c r="BI267" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ267" t="s">
-        <v>65</v>
-      </c>
-      <c r="BK267" t="s">
-        <v>90</v>
-      </c>
-      <c r="BL267" t="s">
-        <v>65</v>
-      </c>
-      <c r="BM267" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN267" t="s">
-        <v>3</v>
+        <v>461</v>
       </c>
     </row>
     <row r="268" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B268" t="s">
-        <v>465</v>
+        <v>463</v>
+      </c>
+      <c r="D268" t="s">
+        <v>36</v>
+      </c>
+      <c r="E268" t="s">
+        <v>35</v>
+      </c>
+      <c r="F268" t="s">
+        <v>37</v>
+      </c>
+      <c r="G268" t="s">
+        <v>38</v>
+      </c>
+      <c r="H268" t="s">
+        <v>39</v>
+      </c>
+      <c r="I268" t="s">
+        <v>40</v>
+      </c>
+      <c r="J268" t="s">
+        <v>41</v>
+      </c>
+      <c r="K268" t="s">
+        <v>42</v>
+      </c>
+      <c r="L268" t="s">
+        <v>43</v>
+      </c>
+      <c r="M268" t="s">
+        <v>44</v>
+      </c>
+      <c r="N268" t="s">
+        <v>45</v>
+      </c>
+      <c r="O268" t="s">
+        <v>35</v>
+      </c>
+      <c r="P268" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q268" t="s">
+        <v>47</v>
+      </c>
+      <c r="R268" t="s">
+        <v>48</v>
+      </c>
+      <c r="S268" t="s">
+        <v>49</v>
+      </c>
+      <c r="T268" t="s">
+        <v>50</v>
+      </c>
+      <c r="U268" t="s">
+        <v>51</v>
+      </c>
+      <c r="V268" t="s">
+        <v>9</v>
+      </c>
+      <c r="W268" t="s">
+        <v>52</v>
+      </c>
+      <c r="X268" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y268" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z268" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA268" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB268" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC268" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD268" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE268" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF268" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG268" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH268" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI268" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ268" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK268" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL268" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM268" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN268" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO268" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP268" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ268" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR268" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS268" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT268" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU268" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV268" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW268" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX268" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY268" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ268" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA268" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB268" t="s">
+        <v>82</v>
+      </c>
+      <c r="BC268" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD268" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE268" t="s">
+        <v>85</v>
+      </c>
+      <c r="BF268" t="s">
+        <v>86</v>
+      </c>
+      <c r="BG268" t="s">
+        <v>87</v>
+      </c>
+      <c r="BH268" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI268" t="s">
+        <v>89</v>
+      </c>
+      <c r="BJ268" t="s">
+        <v>65</v>
+      </c>
+      <c r="BK268" t="s">
+        <v>90</v>
+      </c>
+      <c r="BL268" t="s">
+        <v>65</v>
+      </c>
+      <c r="BM268" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN268" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="269" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
+        <v>464</v>
+      </c>
+      <c r="B269" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="270" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
         <v>466</v>
       </c>
-      <c r="B269" t="s">
+      <c r="B270" t="s">
         <v>467</v>
-      </c>
-    </row>
-    <row r="271" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
-        <v>468</v>
-      </c>
-      <c r="B271" t="s">
-        <v>469</v>
-      </c>
-      <c r="C271" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="272" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B272" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C272" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>471</v>
+      </c>
+      <c r="B273" t="s">
+        <v>472</v>
+      </c>
+      <c r="C273" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
         <v>474</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B274" t="s">
         <v>475</v>
       </c>
-      <c r="C273" t="s">
+      <c r="C274" t="s">
         <v>476</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
-        <v>477</v>
-      </c>
-      <c r="B275" t="s">
-        <v>254</v>
-      </c>
-      <c r="C275" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B276" t="s">
-        <v>480</v>
+        <v>254</v>
       </c>
       <c r="C276" t="s">
-        <v>481</v>
+        <v>255</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B277" t="s">
-        <v>141</v>
+        <v>480</v>
       </c>
       <c r="C277" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B278" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C278" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B279" t="s">
-        <v>487</v>
+        <v>2</v>
       </c>
       <c r="C279" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B280" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="C280" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B281" t="s">
         <v>478</v>
@@ -5703,7 +5721,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B282" t="s">
         <v>478</v>
@@ -5714,7 +5732,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B283" t="s">
         <v>478</v>
@@ -5725,7 +5743,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B284" t="s">
         <v>478</v>
@@ -5736,15 +5754,18 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B285" t="s">
-        <v>480</v>
+        <v>478</v>
+      </c>
+      <c r="C285" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B286" t="s">
         <v>480</v>
@@ -5752,162 +5773,162 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B287" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
+        <v>497</v>
+      </c>
+      <c r="B288" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
         <v>498</v>
-      </c>
-      <c r="B288" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>499</v>
       </c>
       <c r="B289" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
+        <v>499</v>
+      </c>
+      <c r="B290" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
         <v>500</v>
-      </c>
-      <c r="B290" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>501</v>
       </c>
       <c r="B291" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B292" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
+        <v>502</v>
+      </c>
+      <c r="B293" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
         <v>503</v>
-      </c>
-      <c r="B293" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>504</v>
       </c>
       <c r="B294" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
+        <v>504</v>
+      </c>
+      <c r="B295" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
         <v>505</v>
-      </c>
-      <c r="B295" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>506</v>
       </c>
       <c r="B296" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
+        <v>506</v>
+      </c>
+      <c r="B297" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
         <v>507</v>
-      </c>
-      <c r="B297" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>508</v>
       </c>
       <c r="B298" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
+        <v>508</v>
+      </c>
+      <c r="B299" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
         <v>509</v>
-      </c>
-      <c r="B299" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>510</v>
       </c>
       <c r="B300" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
+        <v>510</v>
+      </c>
+      <c r="B301" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
         <v>511</v>
       </c>
-      <c r="B301" t="s">
+      <c r="B302" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
         <v>120</v>
       </c>
-      <c r="B302" t="s">
+      <c r="B303" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
         <v>512</v>
       </c>
-      <c r="B303" t="s">
+      <c r="B304" t="s">
         <v>487</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A304" t="s">
-        <v>513</v>
-      </c>
-      <c r="B304" t="s">
-        <v>93</v>
-      </c>
-      <c r="C304" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B305" t="s">
-        <v>478</v>
+        <v>93</v>
+      </c>
+      <c r="C305" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B306" t="s">
         <v>478</v>
@@ -5915,15 +5936,15 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B307" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B308" t="s">
         <v>480</v>
@@ -5931,7 +5952,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B309" t="s">
         <v>480</v>
@@ -5939,7 +5960,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B310" t="s">
         <v>480</v>
@@ -5947,14 +5968,19 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
+        <v>520</v>
+      </c>
+      <c r="B311" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
         <v>521</v>
       </c>
-      <c r="B311" t="s">
+      <c r="B312" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C313" s="1"/>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C314" s="1"/>
@@ -6022,7 +6048,11 @@
     <row r="335" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C335" s="1"/>
     </row>
+    <row r="336" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C336" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>